<commit_message>
Adding some data. Change the format of citation
</commit_message>
<xml_diff>
--- a/paper/data/scalobility/8node-scalobility.xlsx
+++ b/paper/data/scalobility/8node-scalobility.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinzhao/Library/Mobile Documents/com~apple~CloudDocs/C:C++ project/numalloc/paper/data/scalobility/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tongpingliu/projects/numalloc/paper/data/scalobility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09825EA6-5640-0046-B662-952977132B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D311FC-C86C-F74D-8F42-111C54DF4DC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{3A2DC044-6BB7-684C-8FBF-8D134127710A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{3A2DC044-6BB7-684C-8FBF-8D134127710A}"/>
   </bookViews>
   <sheets>
     <sheet name="regular" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -4596,10 +4594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D94CDA-0228-0544-A979-BC3A7DF19415}">
-  <dimension ref="A1:AE43"/>
+  <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:AE43"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4607,7 +4605,7 @@
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -4691,7 +4689,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -4789,8 +4787,16 @@
         <f>B2/I2</f>
         <v>8.0327557855857972</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AG2">
+        <f>AVERAGE(AE2+AE14+AE26+AE37)</f>
+        <v>114.48180549503709</v>
+      </c>
+      <c r="AH2">
+        <f>AG3/AG2</f>
+        <v>2.2234506055066028</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -4857,39 +4863,47 @@
         <v>51</v>
       </c>
       <c r="X3" s="2">
-        <f t="shared" ref="X3:X9" si="8">B3/B3</f>
+        <f t="shared" ref="X3:X8" si="8">B3/B3</f>
         <v>1</v>
       </c>
       <c r="Y3" s="2">
-        <f t="shared" ref="Y3:Y9" si="9">B3/C3</f>
+        <f t="shared" ref="Y3:Y8" si="9">B3/C3</f>
         <v>2.0366967002320102</v>
       </c>
       <c r="Z3" s="2">
-        <f t="shared" ref="Z3:Z9" si="10">B3/D3</f>
+        <f t="shared" ref="Z3:Z8" si="10">B3/D3</f>
         <v>4.1243354278431417</v>
       </c>
       <c r="AA3" s="2">
-        <f t="shared" ref="AA3:AA9" si="11">B3/E3</f>
+        <f t="shared" ref="AA3:AA8" si="11">B3/E3</f>
         <v>8.6675977655514043</v>
       </c>
       <c r="AB3" s="2">
-        <f t="shared" ref="AB3:AB9" si="12">B3/F3</f>
+        <f t="shared" ref="AB3:AB8" si="12">B3/F3</f>
         <v>17.713025428484809</v>
       </c>
       <c r="AC3" s="2">
-        <f t="shared" ref="AC3:AC9" si="13">B3/G3</f>
+        <f t="shared" ref="AC3:AC8" si="13">B3/G3</f>
         <v>36.584137184154173</v>
       </c>
       <c r="AD3">
-        <f t="shared" ref="AD3:AD9" si="14">B3/H3</f>
+        <f t="shared" ref="AD3:AD8" si="14">B3/H3</f>
         <v>60.412389356382228</v>
       </c>
       <c r="AE3">
-        <f t="shared" ref="AE3:AE8" si="15">B3/I3</f>
+        <f t="shared" ref="AE3:AE7" si="15">B3/I3</f>
         <v>75.851111110755554</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF3">
+        <f>AE3/AE6</f>
+        <v>2.6458310309521642</v>
+      </c>
+      <c r="AG3">
+        <f>AVERAGE(AE3+AE15+AE27+AE38)</f>
+        <v>254.54463974742936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -4987,8 +5001,12 @@
         <f t="shared" si="15"/>
         <v>1.8748744015916996</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AG4">
+        <f>AVERAGE(AE4+AE16+AE28+AE39)</f>
+        <v>18.034562956589824</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5086,8 +5104,12 @@
         <f t="shared" si="15"/>
         <v>1.5131845168900075</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AG5">
+        <f>AVERAGE(AE5+AE17+AE29+AE40)</f>
+        <v>92.13341744253006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5185,8 +5207,12 @@
         <f t="shared" si="15"/>
         <v>28.668161429590139</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AG6">
+        <f>AVERAGE(AE6+AE18+AE30+AE41)</f>
+        <v>116.38900051124044</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -5284,8 +5310,12 @@
         <f t="shared" si="15"/>
         <v>8.1305516443912058</v>
       </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AG7">
+        <f>AVERAGE(AE7+AE19+AE31+AE42)</f>
+        <v>113.14653626650136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -5383,8 +5413,16 @@
         <f>B8/I8</f>
         <v>9.5693274673881241</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AG8">
+        <f>AVERAGE(AE8+AE20+AE32+AE43)</f>
+        <v>142.43270133295098</v>
+      </c>
+      <c r="AH8">
+        <f>AG3/AG8</f>
+        <v>1.7871221802667723</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
@@ -5398,7 +5436,7 @@
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -5419,7 +5457,7 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -5433,7 +5471,7 @@
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -5447,7 +5485,7 @@
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -5530,7 +5568,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -5597,39 +5635,39 @@
         <v>50</v>
       </c>
       <c r="X14" s="2">
-        <f t="shared" ref="X10:X43" si="24">B14/B14</f>
+        <f t="shared" ref="X14:X37" si="24">B14/B14</f>
         <v>1</v>
       </c>
       <c r="Y14" s="2">
-        <f t="shared" ref="Y10:Y43" si="25">B14/C14</f>
+        <f t="shared" ref="Y14:Y32" si="25">B14/C14</f>
         <v>1.9904328017754311</v>
       </c>
       <c r="Z14" s="2">
-        <f t="shared" ref="Z10:Z43" si="26">B14/D14</f>
+        <f t="shared" ref="Z14:Z32" si="26">B14/D14</f>
         <v>0.23305062144065533</v>
       </c>
       <c r="AA14" s="2">
-        <f t="shared" ref="AA10:AA43" si="27">B14/E14</f>
+        <f t="shared" ref="AA14:AA32" si="27">B14/E14</f>
         <v>0.32228082470263908</v>
       </c>
       <c r="AB14" s="2">
-        <f t="shared" ref="AB10:AB43" si="28">B14/F14</f>
+        <f t="shared" ref="AB14:AB32" si="28">B14/F14</f>
         <v>0.58444251221633936</v>
       </c>
       <c r="AC14" s="2">
-        <f t="shared" ref="AC10:AC43" si="29">B14/G14</f>
+        <f t="shared" ref="AC14:AC32" si="29">B14/G14</f>
         <v>0.76347750111848645</v>
       </c>
       <c r="AD14">
-        <f t="shared" ref="AD10:AD43" si="30">B14/H14</f>
+        <f t="shared" ref="AD14:AD32" si="30">B14/H14</f>
         <v>1.4594955737578441</v>
       </c>
       <c r="AE14">
-        <f t="shared" ref="AE9:AE43" si="31">B14/I14</f>
+        <f t="shared" ref="AE14:AE32" si="31">B14/I14</f>
         <v>3.0488485695014718</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -5728,7 +5766,7 @@
         <v>47.270270231817207</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -5827,7 +5865,7 @@
         <v>1.3223415518722477</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -5926,7 +5964,7 @@
         <v>10.306698004963328</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -6025,7 +6063,7 @@
         <v>1.3420850606202328</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -6124,7 +6162,7 @@
         <v>3.1318996418337091</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -6223,7 +6261,7 @@
         <v>48.0329670260342</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -6237,7 +6275,7 @@
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -6251,7 +6289,7 @@
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -6265,7 +6303,7 @@
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -6279,7 +6317,7 @@
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -6362,7 +6400,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -6461,7 +6499,7 @@
         <v>81.612722216670278</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -6559,8 +6597,12 @@
         <f t="shared" si="31"/>
         <v>106.14355227837864</v>
       </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF27">
+        <f>AE27/AE26</f>
+        <v>1.300576054755072</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -6659,7 +6701,7 @@
         <v>1.3426443202913392</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -6758,7 +6800,7 @@
         <v>80.216911744651654</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -6857,7 +6899,7 @@
         <v>76.528070185642335</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -6956,7 +6998,7 @@
         <v>80.039449524835916</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -7055,7 +7097,7 @@
         <v>79.316363636363633</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -7069,7 +7111,7 @@
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -7083,7 +7125,7 @@
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -7097,7 +7139,7 @@
       <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>62</v>
       </c>
@@ -7180,7 +7222,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -7279,7 +7321,7 @@
         <v>21.787478923279558</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -7377,8 +7419,12 @@
         <f t="shared" ref="AE38:AE43" si="55">I38/B38</f>
         <v>25.279706126477944</v>
       </c>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF38">
+        <f>AE38/AE37</f>
+        <v>1.1602859704647608</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -7477,7 +7523,7 @@
         <v>13.494702682834536</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -7576,7 +7622,7 @@
         <v>9.6623176025078E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -7675,7 +7721,7 @@
         <v>9.8506838353877217</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -7774,7 +7820,7 @@
         <v>21.844635455440532</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -7883,8 +7929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9751B6-9DD4-A94E-B89E-DA491D45E4AB}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>